<commit_message>
Add support for deleting sparklines from rows and columns that have been deleted.
</commit_message>
<xml_diff>
--- a/EPPlusTest/Workbooks/Sparkline Demos.xlsx
+++ b/EPPlusTest/Workbooks/Sparkline Demos.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\med\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\med\Source\Repos\EPPlus\EPPlusTest\Workbooks\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -339,7 +339,7 @@
   <dimension ref="D6:F8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -382,6 +382,38 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{05C60535-1F16-4fd2-B633-F4F36F0B64E0}">
       <x14:sparklineGroups xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+        <x14:sparklineGroup type="stacked" displayEmptyCellsAs="gap" negative="1">
+          <x14:colorSeries rgb="FF323232"/>
+          <x14:colorNegative rgb="FFD00000"/>
+          <x14:colorAxis rgb="FF000000"/>
+          <x14:colorMarkers rgb="FFD00000"/>
+          <x14:colorFirst rgb="FFD00000"/>
+          <x14:colorLast rgb="FFD00000"/>
+          <x14:colorHigh rgb="FFD00000"/>
+          <x14:colorLow rgb="FFD00000"/>
+          <x14:sparklines>
+            <x14:sparkline>
+              <xm:f>Sheet1!F6:F8</xm:f>
+              <xm:sqref>F9</xm:sqref>
+            </x14:sparkline>
+          </x14:sparklines>
+        </x14:sparklineGroup>
+        <x14:sparklineGroup displayEmptyCellsAs="gap">
+          <x14:colorSeries rgb="FF376092"/>
+          <x14:colorNegative rgb="FFD00000"/>
+          <x14:colorAxis rgb="FF000000"/>
+          <x14:colorMarkers rgb="FFD00000"/>
+          <x14:colorFirst rgb="FFD00000"/>
+          <x14:colorLast rgb="FFD00000"/>
+          <x14:colorHigh rgb="FFD00000"/>
+          <x14:colorLow rgb="FFD00000"/>
+          <x14:sparklines>
+            <x14:sparkline>
+              <xm:f>Sheet1!E6:E8</xm:f>
+              <xm:sqref>E9</xm:sqref>
+            </x14:sparkline>
+          </x14:sparklines>
+        </x14:sparklineGroup>
         <x14:sparklineGroup type="column" displayEmptyCellsAs="gap">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
@@ -393,40 +425,56 @@
           <x14:colorLow rgb="FFD00000"/>
           <x14:sparklines>
             <x14:sparkline>
+              <xm:f>Sheet1!D6:D8</xm:f>
+              <xm:sqref>D9</xm:sqref>
+            </x14:sparkline>
+          </x14:sparklines>
+        </x14:sparklineGroup>
+        <x14:sparklineGroup type="stacked" displayEmptyCellsAs="gap" negative="1">
+          <x14:colorSeries rgb="FF323232"/>
+          <x14:colorNegative rgb="FFD00000"/>
+          <x14:colorAxis rgb="FF000000"/>
+          <x14:colorMarkers rgb="FFD00000"/>
+          <x14:colorFirst rgb="FFD00000"/>
+          <x14:colorLast rgb="FFD00000"/>
+          <x14:colorHigh rgb="FFD00000"/>
+          <x14:colorLow rgb="FFD00000"/>
+          <x14:sparklines>
+            <x14:sparkline>
+              <xm:f>Sheet1!D8:F8</xm:f>
+              <xm:sqref>G8</xm:sqref>
+            </x14:sparkline>
+          </x14:sparklines>
+        </x14:sparklineGroup>
+        <x14:sparklineGroup displayEmptyCellsAs="gap">
+          <x14:colorSeries rgb="FF376092"/>
+          <x14:colorNegative rgb="FFD00000"/>
+          <x14:colorAxis rgb="FF000000"/>
+          <x14:colorMarkers rgb="FFD00000"/>
+          <x14:colorFirst rgb="FFD00000"/>
+          <x14:colorLast rgb="FFD00000"/>
+          <x14:colorHigh rgb="FFD00000"/>
+          <x14:colorLow rgb="FFD00000"/>
+          <x14:sparklines>
+            <x14:sparkline>
+              <xm:f>Sheet1!D7:F7</xm:f>
+              <xm:sqref>G7</xm:sqref>
+            </x14:sparkline>
+          </x14:sparklines>
+        </x14:sparklineGroup>
+        <x14:sparklineGroup type="column" displayEmptyCellsAs="gap">
+          <x14:colorSeries rgb="FF376092"/>
+          <x14:colorNegative rgb="FFD00000"/>
+          <x14:colorAxis rgb="FF000000"/>
+          <x14:colorMarkers rgb="FFD00000"/>
+          <x14:colorFirst rgb="FFD00000"/>
+          <x14:colorLast rgb="FFD00000"/>
+          <x14:colorHigh rgb="FFD00000"/>
+          <x14:colorLow rgb="FFD00000"/>
+          <x14:sparklines>
+            <x14:sparkline>
               <xm:f>Sheet1!D6:F6</xm:f>
               <xm:sqref>G6</xm:sqref>
-            </x14:sparkline>
-          </x14:sparklines>
-        </x14:sparklineGroup>
-        <x14:sparklineGroup displayEmptyCellsAs="gap">
-          <x14:colorSeries rgb="FF376092"/>
-          <x14:colorNegative rgb="FFD00000"/>
-          <x14:colorAxis rgb="FF000000"/>
-          <x14:colorMarkers rgb="FFD00000"/>
-          <x14:colorFirst rgb="FFD00000"/>
-          <x14:colorLast rgb="FFD00000"/>
-          <x14:colorHigh rgb="FFD00000"/>
-          <x14:colorLow rgb="FFD00000"/>
-          <x14:sparklines>
-            <x14:sparkline>
-              <xm:f>Sheet1!D7:F7</xm:f>
-              <xm:sqref>G7</xm:sqref>
-            </x14:sparkline>
-          </x14:sparklines>
-        </x14:sparklineGroup>
-        <x14:sparklineGroup type="stacked" displayEmptyCellsAs="gap" negative="1">
-          <x14:colorSeries rgb="FF323232"/>
-          <x14:colorNegative rgb="FFD00000"/>
-          <x14:colorAxis rgb="FF000000"/>
-          <x14:colorMarkers rgb="FFD00000"/>
-          <x14:colorFirst rgb="FFD00000"/>
-          <x14:colorLast rgb="FFD00000"/>
-          <x14:colorHigh rgb="FFD00000"/>
-          <x14:colorLow rgb="FFD00000"/>
-          <x14:sparklines>
-            <x14:sparkline>
-              <xm:f>Sheet1!D8:F8</xm:f>
-              <xm:sqref>G8</xm:sqref>
             </x14:sparkline>
           </x14:sparklines>
         </x14:sparklineGroup>

</xml_diff>

<commit_message>
Updates sparkline cross-sheet formula implementation, adds sparkline tests.
</commit_message>
<xml_diff>
--- a/EPPlusTest/Workbooks/Sparkline Demos.xlsx
+++ b/EPPlusTest/Workbooks/Sparkline Demos.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\med\Source\Repos\EPPlus\EPPlusTest\Workbooks\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Source\EPPlus\EPPlusTest\Workbooks\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -13,6 +13,7 @@
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913" calcMode="manual" concurrentManualCount="1"/>
   <extLst>
@@ -54,7 +55,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
@@ -339,7 +341,7 @@
   <dimension ref="D6:F8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -478,8 +480,65 @@
             </x14:sparkline>
           </x14:sparklines>
         </x14:sparklineGroup>
+        <x14:sparklineGroup displayEmptyCellsAs="gap">
+          <x14:colorSeries rgb="FF376092"/>
+          <x14:colorNegative rgb="FFD00000"/>
+          <x14:colorAxis rgb="FF000000"/>
+          <x14:colorMarkers rgb="FFD00000"/>
+          <x14:colorFirst rgb="FFD00000"/>
+          <x14:colorLast rgb="FFD00000"/>
+          <x14:colorHigh rgb="FFD00000"/>
+          <x14:colorLow rgb="FFD00000"/>
+          <x14:sparklines>
+            <x14:sparkline>
+              <xm:f>Sheet2!B2:I2</xm:f>
+              <xm:sqref>C12</xm:sqref>
+            </x14:sparkline>
+          </x14:sparklines>
+        </x14:sparklineGroup>
       </x14:sparklineGroups>
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:I2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="2" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B2" s="1">
+        <v>43.5</v>
+      </c>
+      <c r="C2" s="1">
+        <v>43.3</v>
+      </c>
+      <c r="D2" s="1">
+        <v>43.1</v>
+      </c>
+      <c r="E2" s="1">
+        <v>44.1</v>
+      </c>
+      <c r="F2" s="1">
+        <v>43.8</v>
+      </c>
+      <c r="G2" s="1">
+        <v>44.4</v>
+      </c>
+      <c r="H2" s="1">
+        <v>44.7</v>
+      </c>
+      <c r="I2" s="1">
+        <v>44.7</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Adds support and tests for cross-sheet sparklines. (#106)
* Adds support and tests for cross-sheet sparklines.

* Updates sparkline cross-sheet formula implementation, adds sparkline tests.

* Updates sparklines and related tests for bug fix and pr comments.

* Fixes corrupting workbooks without sparklines.
</commit_message>
<xml_diff>
--- a/EPPlusTest/Workbooks/Sparkline Demos.xlsx
+++ b/EPPlusTest/Workbooks/Sparkline Demos.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\med\Source\Repos\EPPlus\EPPlusTest\Workbooks\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Source\EPPlus\EPPlusTest\Workbooks\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -13,6 +13,7 @@
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913" calcMode="manual" concurrentManualCount="1"/>
   <extLst>
@@ -54,7 +55,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
@@ -339,7 +341,7 @@
   <dimension ref="D6:F8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -478,8 +480,65 @@
             </x14:sparkline>
           </x14:sparklines>
         </x14:sparklineGroup>
+        <x14:sparklineGroup displayEmptyCellsAs="gap">
+          <x14:colorSeries rgb="FF376092"/>
+          <x14:colorNegative rgb="FFD00000"/>
+          <x14:colorAxis rgb="FF000000"/>
+          <x14:colorMarkers rgb="FFD00000"/>
+          <x14:colorFirst rgb="FFD00000"/>
+          <x14:colorLast rgb="FFD00000"/>
+          <x14:colorHigh rgb="FFD00000"/>
+          <x14:colorLow rgb="FFD00000"/>
+          <x14:sparklines>
+            <x14:sparkline>
+              <xm:f>Sheet2!B2:I2</xm:f>
+              <xm:sqref>C12</xm:sqref>
+            </x14:sparkline>
+          </x14:sparklines>
+        </x14:sparklineGroup>
       </x14:sparklineGroups>
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:I2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="2" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B2" s="1">
+        <v>43.5</v>
+      </c>
+      <c r="C2" s="1">
+        <v>43.3</v>
+      </c>
+      <c r="D2" s="1">
+        <v>43.1</v>
+      </c>
+      <c r="E2" s="1">
+        <v>44.1</v>
+      </c>
+      <c r="F2" s="1">
+        <v>43.8</v>
+      </c>
+      <c r="G2" s="1">
+        <v>44.4</v>
+      </c>
+      <c r="H2" s="1">
+        <v>44.7</v>
+      </c>
+      <c r="I2" s="1">
+        <v>44.7</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>